<commit_message>
update file paths in spreadsheets to "resources/stimuli"
</commit_message>
<xml_diff>
--- a/html/resources/1condition/practice.xlsx
+++ b/html/resources/1condition/practice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janet/Desktop/Sinai_Projects/Code/fish-task-6B20T-practice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janet/Desktop/Sinai_Projects/Code/fish-task-6B20T/html/resources/1condition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF572E27-29BA-1742-9AD3-ED896E5CDD6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B82C28-39CC-0144-AB98-0CB2016A8404}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8260" yWindow="1160" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,19 +62,19 @@
     <t>right</t>
   </si>
   <si>
-    <t>stimuli/bead_y.PNG</t>
-  </si>
-  <si>
-    <t>stimuli/blank.JPG</t>
-  </si>
-  <si>
-    <t>stimuli/bead_b.PNG</t>
-  </si>
-  <si>
-    <t>stimuli/bead_g.PNG</t>
-  </si>
-  <si>
     <t>up</t>
+  </si>
+  <si>
+    <t>resources/stimuli/bead_y.PNG</t>
+  </si>
+  <si>
+    <t>resources/stimuli/blank.JPG</t>
+  </si>
+  <si>
+    <t>resources/stimuli/bead_b.PNG</t>
+  </si>
+  <si>
+    <t>resources/stimuli/bead_g.PNG</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -442,28 +442,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -471,31 +471,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -503,19 +503,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -525,10 +525,10 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -536,19 +536,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -558,10 +558,10 @@
         <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -569,19 +569,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -591,10 +591,10 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -602,19 +602,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -624,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -632,19 +632,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -654,7 +654,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -662,19 +662,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -684,7 +684,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -692,19 +692,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -722,19 +722,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -744,7 +744,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -752,19 +752,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -781,19 +781,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -810,19 +810,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -839,19 +839,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -868,19 +868,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -897,19 +897,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -926,19 +926,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -955,19 +955,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -984,19 +984,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G20">
         <v>2</v>
@@ -1013,19 +1013,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G21">
         <v>2</v>

</xml_diff>

<commit_message>
Change practice excel back to original file paths
</commit_message>
<xml_diff>
--- a/html/resources/1condition/practice.xlsx
+++ b/html/resources/1condition/practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janet/Desktop/Sinai_Projects/Code/fish-task-6B20T/html/resources/1condition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B82C28-39CC-0144-AB98-0CB2016A8404}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2031CA-7003-4C4D-B5D6-C7F18611E913}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8260" yWindow="1160" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,19 +62,19 @@
     <t>right</t>
   </si>
   <si>
+    <t>stimuli/bead_y.PNG</t>
+  </si>
+  <si>
+    <t>stimuli/blank.JPG</t>
+  </si>
+  <si>
+    <t>stimuli/bead_b.PNG</t>
+  </si>
+  <si>
+    <t>stimuli/bead_g.PNG</t>
+  </si>
+  <si>
     <t>up</t>
-  </si>
-  <si>
-    <t>resources/stimuli/bead_y.PNG</t>
-  </si>
-  <si>
-    <t>resources/stimuli/blank.JPG</t>
-  </si>
-  <si>
-    <t>resources/stimuli/bead_b.PNG</t>
-  </si>
-  <si>
-    <t>resources/stimuli/bead_g.PNG</t>
   </si>
 </sst>
 </file>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -442,19 +442,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -471,19 +471,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -492,10 +492,10 @@
         <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -503,19 +503,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -525,10 +525,10 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -536,19 +536,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -558,10 +558,10 @@
         <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -569,19 +569,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -591,10 +591,10 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -602,19 +602,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -624,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -632,19 +632,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -654,7 +654,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -662,19 +662,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -684,7 +684,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -692,19 +692,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -722,19 +722,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -744,7 +744,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -752,19 +752,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -781,19 +781,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -810,19 +810,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -839,19 +839,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -868,19 +868,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -897,19 +897,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -926,19 +926,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -955,19 +955,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -984,19 +984,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G20">
         <v>2</v>
@@ -1013,19 +1013,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21">
         <v>2</v>

</xml_diff>

<commit_message>
change jpg capitalization in conditions files
</commit_message>
<xml_diff>
--- a/html/resources/1condition/practice.xlsx
+++ b/html/resources/1condition/practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janet/Desktop/Sinai_Projects/Code/fish-task-6B20T/html/resources/1condition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2031CA-7003-4C4D-B5D6-C7F18611E913}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C812C0BB-87D3-004B-8217-3DB102B25363}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8260" yWindow="1160" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>stimuli/bead_y.PNG</t>
   </si>
   <si>
-    <t>stimuli/blank.JPG</t>
-  </si>
-  <si>
     <t>stimuli/bead_b.PNG</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>up</t>
+  </si>
+  <si>
+    <t>stimuli/blank.jpg</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -445,16 +445,16 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -477,13 +477,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -492,10 +492,10 @@
         <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -512,10 +512,10 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -525,10 +525,10 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -536,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -548,7 +548,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -558,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
@@ -572,7 +572,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -591,10 +591,10 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -608,7 +608,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -624,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -641,7 +641,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -654,7 +654,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -662,7 +662,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -674,7 +674,7 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -684,7 +684,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -728,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -744,7 +744,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -752,7 +752,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -761,7 +761,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -781,10 +781,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -793,7 +793,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -810,13 +810,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -839,16 +839,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
@@ -871,16 +871,16 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -897,19 +897,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -926,19 +926,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -955,19 +955,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -984,16 +984,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
@@ -1013,19 +1013,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G21">
         <v>2</v>

</xml_diff>